<commit_message>
Added everthing up to week 4 (really this time)
</commit_message>
<xml_diff>
--- a/wk2/HW_2_Isaacson.xlsx
+++ b/wk2/HW_2_Isaacson.xlsx
@@ -20,15 +20,56 @@
   <definedNames>
     <definedName name="BatchesProduced">'3.5-3'!$D$10:$F$10</definedName>
     <definedName name="Cost">'3.5-6'!$D$3:$F$3</definedName>
+    <definedName name="grb_async_callbacks" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="grb_bariter" localSheetId="3" hidden="1">1E+100</definedName>
+    <definedName name="grb_bartol" localSheetId="3" hidden="1">0.00000001</definedName>
+    <definedName name="grb_crossover" localSheetId="3" hidden="1">-1</definedName>
+    <definedName name="grb_cut_passes" localSheetId="3" hidden="1">-1</definedName>
+    <definedName name="grb_cutoff" localSheetId="3" hidden="1">1E+100</definedName>
+    <definedName name="grb_cuts" localSheetId="3" hidden="1">-1</definedName>
+    <definedName name="grb_focus" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="grb_heur" localSheetId="3" hidden="1">0.05</definedName>
+    <definedName name="grb_improv" localSheetId="3" hidden="1">1E+100</definedName>
+    <definedName name="grb_improv_start_gap" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="grb_infeas" localSheetId="3" hidden="1">0.000001</definedName>
+    <definedName name="grb_inttol" localSheetId="3" hidden="1">0.00001</definedName>
+    <definedName name="grb_method" localSheetId="3" hidden="1">-1</definedName>
+    <definedName name="grb_nodefilestart" localSheetId="3" hidden="1">1E+100</definedName>
+    <definedName name="grb_optimal" localSheetId="3" hidden="1">0.000001</definedName>
+    <definedName name="grb_order" localSheetId="3" hidden="1">-1</definedName>
+    <definedName name="grb_pre_passes" localSheetId="3" hidden="1">-1</definedName>
+    <definedName name="grb_presolve" localSheetId="3" hidden="1">-1</definedName>
+    <definedName name="grb_pricing" localSheetId="3" hidden="1">-1</definedName>
+    <definedName name="grb_psdtol" localSheetId="3" hidden="1">0.000001</definedName>
+    <definedName name="grb_qcptol" localSheetId="3" hidden="1">0.000001</definedName>
+    <definedName name="grb_relmip" localSheetId="3" hidden="1">0.0001</definedName>
+    <definedName name="grb_scaleflag" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="grb_seed" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="grb_submip" localSheetId="3" hidden="1">500</definedName>
+    <definedName name="grb_symmetry" localSheetId="3" hidden="1">-1</definedName>
+    <definedName name="grb_threads" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="grb_var" localSheetId="3" hidden="1">-1</definedName>
+    <definedName name="grb_zeroobjnodes" localSheetId="3" hidden="1">-1</definedName>
+    <definedName name="gurobi_qp" localSheetId="3" hidden="1">0</definedName>
     <definedName name="ProfitPerBatch">'3.5-3'!$D$3:$F$3</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'3.4-10'!$C$12:$I$12</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">'3.4-15'!$C$22:$AF$22</definedName>
     <definedName name="solver_adj" localSheetId="2" hidden="1">'3.5-3'!$D$10:$F$10</definedName>
     <definedName name="solver_adj" localSheetId="3" hidden="1">'3.5-6'!$D$11:$F$11</definedName>
+    <definedName name="solver_adj_ob" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_cha" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_chc1" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_chn" localSheetId="3" hidden="1">4</definedName>
+    <definedName name="solver_chp1" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_cht" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_cir1" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_con" localSheetId="3" hidden="1">" "</definedName>
+    <definedName name="solver_con1" localSheetId="3" hidden="1">" "</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
+    <definedName name="solver_dia" localSheetId="3" hidden="1">5</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
@@ -36,15 +77,20 @@
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_eng" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">6</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_iao" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_int" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_irs" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_ism" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs_ob1" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'3.4-10'!$C$12:$I$12</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">'3.4-15'!$C$22:$AF$22</definedName>
     <definedName name="solver_lhs1" localSheetId="2" hidden="1">'3.5-3'!$G$6:$G$7</definedName>
@@ -56,6 +102,8 @@
     <definedName name="solver_lhs4" localSheetId="1" hidden="1">'3.4-15'!#REF!</definedName>
     <definedName name="solver_lhs5" localSheetId="1" hidden="1">'3.4-15'!#REF!</definedName>
     <definedName name="solver_lhs6" localSheetId="1" hidden="1">'3.4-15'!$C$22:$AF$22</definedName>
+    <definedName name="solver_lin" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_mda" localSheetId="3" hidden="1">4</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
@@ -64,6 +112,7 @@
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
+    <definedName name="solver_mod" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
@@ -80,6 +129,8 @@
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_ntr" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_ntri" hidden="1">1000</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">1</definedName>
@@ -88,18 +139,24 @@
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_obc" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_obp" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'3.4-10'!$L$12</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">'3.4-15'!$AH$22</definedName>
     <definedName name="solver_opt" localSheetId="2" hidden="1">'3.5-3'!$I$10</definedName>
     <definedName name="solver_opt" localSheetId="3" hidden="1">'3.5-6'!$I$11</definedName>
+    <definedName name="solver_opt_ob" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
+    <definedName name="solver_psi" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rdp" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_reco1" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="2" hidden="1">1</definedName>
@@ -111,6 +168,7 @@
     <definedName name="solver_rel4" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel5" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel6" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rep" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">integer</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">'3.4-15'!$C$21:$AF$21</definedName>
     <definedName name="solver_rhs1" localSheetId="2" hidden="1">'3.5-3'!$I$6:$I$7</definedName>
@@ -125,19 +183,29 @@
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_rsmp" hidden="1">2</definedName>
+    <definedName name="solver_rtr" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_rxc1" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rxv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_seed" hidden="1">0</definedName>
+    <definedName name="solver_sel" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_slv" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_slvu" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_spid" localSheetId="3" hidden="1">" "</definedName>
+    <definedName name="solver_srvr" localSheetId="3" hidden="1">" "</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
@@ -154,14 +222,21 @@
     <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_umod" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_urs" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_userid" localSheetId="3" hidden="1">319624</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_var" localSheetId="3" hidden="1">" "</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">16</definedName>
+    <definedName name="solver_vir" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_vol" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_vst" localSheetId="3" hidden="1">0</definedName>
     <definedName name="TotalCost">'3.5-6'!$I$11</definedName>
     <definedName name="Units">'3.5-6'!$D$11:$F$11</definedName>
   </definedNames>
@@ -580,10 +655,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -905,19 +980,19 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -943,7 +1018,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -969,7 +1044,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="N5" t="s">
         <v>16</v>
       </c>
@@ -980,7 +1055,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -1018,7 +1093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -1058,7 +1133,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -1098,7 +1173,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -1136,7 +1211,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>13</v>
       </c>
@@ -1179,115 +1254,115 @@
       <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="32" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="32" width="3.73046875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="13" t="s">
+      <c r="J2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="O2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="P2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="Q2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="R2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="S2" s="13" t="s">
+      <c r="S2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="T2" s="13" t="s">
+      <c r="T2" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="U2" s="13" t="s">
+      <c r="U2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="V2" s="13" t="s">
+      <c r="V2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="W2" s="13" t="s">
+      <c r="W2" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="X2" s="13" t="s">
+      <c r="X2" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="Y2" s="13" t="s">
+      <c r="Y2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="Z2" s="13" t="s">
+      <c r="Z2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AA2" s="13" t="s">
+      <c r="AA2" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="AB2" s="13" t="s">
+      <c r="AB2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="AC2" s="13" t="s">
+      <c r="AC2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="AD2" s="13" t="s">
+      <c r="AD2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="AE2" s="13" t="s">
+      <c r="AE2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="AF2" s="13" t="s">
+      <c r="AF2" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>71</v>
       </c>
@@ -1382,7 +1457,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.45">
       <c r="AG4" s="10"/>
       <c r="AH4" s="10"/>
       <c r="AI4" s="10"/>
@@ -1392,7 +1467,7 @@
       <c r="AM4" s="10"/>
       <c r="AN4" s="10"/>
     </row>
-    <row r="5" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" hidden="1" x14ac:dyDescent="0.45">
       <c r="AG5" s="10"/>
       <c r="AH5" s="10"/>
       <c r="AI5" s="10"/>
@@ -1402,7 +1477,7 @@
       <c r="AM5" s="10"/>
       <c r="AN5" s="10"/>
     </row>
-    <row r="6" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" hidden="1" x14ac:dyDescent="0.45">
       <c r="B6" s="9" t="s">
         <v>41</v>
       </c>
@@ -1481,7 +1556,7 @@
       <c r="AM6" s="10"/>
       <c r="AN6" s="10"/>
     </row>
-    <row r="7" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" hidden="1" x14ac:dyDescent="0.45">
       <c r="B7" s="9" t="s">
         <v>42</v>
       </c>
@@ -1560,7 +1635,7 @@
       <c r="AM7" s="10"/>
       <c r="AN7" s="10"/>
     </row>
-    <row r="8" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" hidden="1" x14ac:dyDescent="0.45">
       <c r="B8" s="9" t="s">
         <v>43</v>
       </c>
@@ -1639,7 +1714,7 @@
       <c r="AM8" s="10"/>
       <c r="AN8" s="10"/>
     </row>
-    <row r="9" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" hidden="1" x14ac:dyDescent="0.45">
       <c r="B9" s="9" t="s">
         <v>44</v>
       </c>
@@ -1718,7 +1793,7 @@
       <c r="AM9" s="10"/>
       <c r="AN9" s="10"/>
     </row>
-    <row r="10" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" hidden="1" x14ac:dyDescent="0.45">
       <c r="B10" s="9" t="s">
         <v>45</v>
       </c>
@@ -1797,7 +1872,7 @@
       <c r="AM10" s="10"/>
       <c r="AN10" s="10"/>
     </row>
-    <row r="11" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" hidden="1" x14ac:dyDescent="0.45">
       <c r="B11" s="9" t="s">
         <v>46</v>
       </c>
@@ -1876,7 +1951,7 @@
       <c r="AM11" s="10"/>
       <c r="AN11" s="10"/>
     </row>
-    <row r="12" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" hidden="1" x14ac:dyDescent="0.45">
       <c r="B12" s="9" t="s">
         <v>47</v>
       </c>
@@ -1955,7 +2030,7 @@
       <c r="AM12" s="10"/>
       <c r="AN12" s="10"/>
     </row>
-    <row r="13" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" hidden="1" x14ac:dyDescent="0.45">
       <c r="B13" s="9" t="s">
         <v>48</v>
       </c>
@@ -2034,7 +2109,7 @@
       <c r="AM13" s="10"/>
       <c r="AN13" s="10"/>
     </row>
-    <row r="14" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" hidden="1" x14ac:dyDescent="0.45">
       <c r="B14" s="9" t="s">
         <v>49</v>
       </c>
@@ -2113,7 +2188,7 @@
       <c r="AM14" s="10"/>
       <c r="AN14" s="10"/>
     </row>
-    <row r="15" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" hidden="1" x14ac:dyDescent="0.45">
       <c r="B15" s="9" t="s">
         <v>50</v>
       </c>
@@ -2192,7 +2267,7 @@
       <c r="AM15" s="10"/>
       <c r="AN15" s="10"/>
     </row>
-    <row r="16" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" hidden="1" x14ac:dyDescent="0.45">
       <c r="B16" s="9" t="s">
         <v>51</v>
       </c>
@@ -2271,7 +2346,7 @@
       <c r="AM16" s="10"/>
       <c r="AN16" s="10"/>
     </row>
-    <row r="17" spans="2:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:40" hidden="1" x14ac:dyDescent="0.45">
       <c r="B17" s="9" t="s">
         <v>52</v>
       </c>
@@ -2350,7 +2425,7 @@
       <c r="AM17" s="10"/>
       <c r="AN17" s="10"/>
     </row>
-    <row r="18" spans="2:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:40" hidden="1" x14ac:dyDescent="0.45">
       <c r="B18" s="9" t="s">
         <v>53</v>
       </c>
@@ -2429,7 +2504,7 @@
       <c r="AM18" s="10"/>
       <c r="AN18" s="10"/>
     </row>
-    <row r="19" spans="2:40" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:40" hidden="1" x14ac:dyDescent="0.45">
       <c r="B19" s="9" t="s">
         <v>54</v>
       </c>
@@ -2508,7 +2583,7 @@
       <c r="AM19" s="10"/>
       <c r="AN19" s="10"/>
     </row>
-    <row r="20" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:40" x14ac:dyDescent="0.45">
       <c r="AG20" s="10"/>
       <c r="AH20" s="10"/>
       <c r="AI20" s="10"/>
@@ -2518,7 +2593,7 @@
       <c r="AM20" s="10"/>
       <c r="AN20" s="10"/>
     </row>
-    <row r="21" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B21" s="9" t="s">
         <v>75</v>
       </c>
@@ -2621,7 +2696,7 @@
       <c r="AM21" s="10"/>
       <c r="AN21" s="10"/>
     </row>
-    <row r="22" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
         <v>13</v>
       </c>
@@ -2721,7 +2796,7 @@
         <v>1755</v>
       </c>
     </row>
-    <row r="24" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:40" x14ac:dyDescent="0.45">
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
@@ -2737,7 +2812,7 @@
       <c r="O24" s="9"/>
       <c r="P24" s="9"/>
     </row>
-    <row r="25" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B25" s="8" t="s">
         <v>61</v>
       </c>
@@ -2760,7 +2835,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B26" s="8" t="s">
         <v>68</v>
       </c>
@@ -2789,7 +2864,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B27" s="8" t="s">
         <v>69</v>
       </c>
@@ -2812,10 +2887,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B28" s="8"/>
     </row>
-    <row r="29" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B29" s="8" t="s">
         <v>72</v>
       </c>
@@ -2835,7 +2910,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B30" s="8" t="s">
         <v>73</v>
       </c>
@@ -2860,7 +2935,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B31" s="8" t="s">
         <v>74</v>
       </c>
@@ -2880,73 +2955,73 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:40" x14ac:dyDescent="0.45">
       <c r="B32" s="8"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B33" s="8"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B34" s="8"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B35" s="8"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B36" s="8"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B37" s="8"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B38" s="8"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B39" s="8"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B40" s="8"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B41" s="8"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B42" s="8"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B43" s="8"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B44" s="8"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B45" s="8"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B46" s="8"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B47" s="8"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B48" s="8"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B49" s="8"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B50" s="8"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B51" s="8"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B52" s="8"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B53" s="8"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B54" s="8"/>
     </row>
   </sheetData>
@@ -2962,21 +3037,21 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.59765625" customWidth="1"/>
     <col min="8" max="8" width="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D2" t="s">
         <v>85</v>
       </c>
@@ -2987,7 +3062,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C3" t="s">
         <v>80</v>
       </c>
@@ -3001,7 +3076,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G4" t="s">
         <v>82</v>
       </c>
@@ -3009,12 +3084,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D5" s="12" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D5" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
       <c r="G5" t="s">
         <v>83</v>
       </c>
@@ -3022,7 +3097,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
         <v>87</v>
       </c>
@@ -3046,7 +3121,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C7" t="s">
         <v>88</v>
       </c>
@@ -3070,12 +3145,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C10" t="s">
         <v>79</v>
       </c>
@@ -3109,21 +3184,21 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.59765625" customWidth="1"/>
     <col min="8" max="8" width="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D2" t="s">
         <v>92</v>
       </c>
@@ -3134,7 +3209,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C3" t="s">
         <v>98</v>
       </c>
@@ -3148,7 +3223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G4" t="s">
         <v>100</v>
       </c>
@@ -3156,15 +3231,15 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
       <c r="G5" t="s">
         <v>101</v>
       </c>
@@ -3172,7 +3247,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C6">
         <v>5</v>
       </c>
@@ -3196,7 +3271,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C7">
         <v>10</v>
       </c>
@@ -3220,7 +3295,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C8">
         <v>15</v>
       </c>
@@ -3244,12 +3319,12 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C11" t="s">
         <v>99</v>
       </c>

</xml_diff>